<commit_message>
outdoor plants image changes
</commit_message>
<xml_diff>
--- a/data/Outdoor plants (2).xlsx
+++ b/data/Outdoor plants (2).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97333\Desktop\Hawra\Cloud Computing\ITCC481\Landscaping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2753" documentId="13_ncr:1_{72A03CF0-B8FA-4FA0-8DEF-3E82B542A124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6C3F5B8-0082-4B6B-BE85-13E3A93ED540}"/>
+  <xr:revisionPtr revIDLastSave="2809" documentId="13_ncr:1_{72A03CF0-B8FA-4FA0-8DEF-3E82B542A124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25F0C26E-D342-48F4-87D2-05A80780BF19}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8B519764-563C-4CD5-B8E9-9B8B0702B21B}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="512">
   <si>
     <t>Plant ID</t>
   </si>
@@ -117,7 +117,7 @@
     <t>Open Image</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/SK2NM8jh/Euonymus-japonicus-Variegata.jpg</t>
+    <t>https://i.postimg.cc/cHqp41Vb/pexels-theshuttervision-12551940.jpg</t>
   </si>
   <si>
     <t>Shrubs</t>
@@ -165,7 +165,7 @@
     <t>Spider Plant</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/QdndCS8m/Chlorophytum-comosum.jpg</t>
+    <t>https://i.postimg.cc/sx8ngwLc/Chlorophytum-comosum.jpg</t>
   </si>
   <si>
     <t>Herbs</t>
@@ -228,7 +228,7 @@
     <t>Crown of Thorns</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/RV4FDNp7/Euphorbia-milii.jpg</t>
+    <t>https://i.postimg.cc/Gp95FQ7K/Crown-of-Thorns.jpg</t>
   </si>
   <si>
     <t>1 - 1.5 m</t>
@@ -249,7 +249,7 @@
     <t>Aloe vera</t>
   </si>
   <si>
-    <t>https://i.postimg.cc/59wygwg9/Aloe-vera.jpg</t>
+    <t>https://i.postimg.cc/MTwxdNhP/Aloe-vera.jpg</t>
   </si>
   <si>
     <t>0.6 - 1 m</t>
@@ -1492,6 +1492,27 @@
   </si>
   <si>
     <t>1,200-2,000g/year</t>
+  </si>
+  <si>
+    <t>OP-067</t>
+  </si>
+  <si>
+    <t>Mesembryanthemum cordifolium L.f.</t>
+  </si>
+  <si>
+    <t>Baby Sun Rose</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/xX6mmxDf/Mesembryanthemum-cordifolium.jpg</t>
+  </si>
+  <si>
+    <t>0.1 - 0.15 m</t>
+  </si>
+  <si>
+    <t>0.5-2g/year</t>
+  </si>
+  <si>
+    <t>1-4g/year</t>
   </si>
   <si>
     <t>Location type</t>
@@ -1660,7 +1681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1724,6 +1745,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -2073,17 +2100,17 @@
   <dimension ref="A1:U197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="A4:XFD4 A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="25.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" style="4" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
@@ -2102,7 +2129,7 @@
     <col min="22" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" ht="29.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2142,7 +2169,7 @@
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="31" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -2167,68 +2194,68 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:21" s="32" customFormat="1">
+      <c r="A2" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="4" t="s">
+      <c r="L2" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="4" t="s">
+      <c r="P2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" s="4" t="s">
+      <c r="S2" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="32" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2297,68 +2324,68 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:21" s="32" customFormat="1">
+      <c r="A4" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="H4" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" s="4" t="s">
+      <c r="M4" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="S4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T4" s="4" t="s">
+      <c r="S4" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="T4" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="U4" s="32" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5222,7 +5249,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="43.5">
+    <row r="49" spans="1:21">
       <c r="A49" s="4" t="s">
         <v>363</v>
       </c>
@@ -5613,68 +5640,68 @@
         <v>389</v>
       </c>
     </row>
-    <row r="55" spans="1:21">
-      <c r="A55" s="4" t="s">
+    <row r="55" spans="1:21" s="32" customFormat="1">
+      <c r="A55" s="32" t="s">
         <v>400</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="32" t="s">
         <v>401</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="32" t="s">
         <v>402</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D55" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E55" s="34" t="s">
         <v>403</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F55" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="G55" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="H55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I55" s="4" t="s">
+      <c r="H55" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="I55" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="J55" s="4" t="s">
+      <c r="J55" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="K55" s="4" t="s">
+      <c r="K55" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="L55" s="4" t="s">
+      <c r="L55" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="M55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N55" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="O55" s="4" t="s">
+      <c r="M55" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="N55" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="O55" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="P55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q55" s="4" t="s">
+      <c r="P55" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q55" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="R55" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="S55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T55" s="4" t="s">
+      <c r="R55" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="S55" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="T55" s="32" t="s">
         <v>404</v>
       </c>
-      <c r="U55" s="4" t="s">
+      <c r="U55" s="32" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6458,7 +6485,71 @@
         <v>483</v>
       </c>
     </row>
-    <row r="68" spans="1:21"/>
+    <row r="68" spans="1:21" s="32" customFormat="1">
+      <c r="A68" s="32" t="s">
+        <v>484</v>
+      </c>
+      <c r="B68" s="32" t="s">
+        <v>485</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>486</v>
+      </c>
+      <c r="D68" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="E68" s="33" t="s">
+        <v>487</v>
+      </c>
+      <c r="F68" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="G68" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H68" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="I68" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="J68" s="32" t="s">
+        <v>488</v>
+      </c>
+      <c r="K68" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="L68" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="M68" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="N68" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="O68" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="P68" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q68" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="R68" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="S68" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="T68" s="32" t="s">
+        <v>489</v>
+      </c>
+      <c r="U68" s="32" t="s">
+        <v>490</v>
+      </c>
+    </row>
     <row r="69" spans="1:21"/>
     <row r="70" spans="1:21"/>
     <row r="71" spans="1:21"/>
@@ -6753,6 +6844,8 @@
     <hyperlink ref="E34" r:id="rId130" xr:uid="{335A8E87-D725-4028-9DB7-E8624E6E544C}"/>
     <hyperlink ref="E45" r:id="rId131" xr:uid="{B9227BF6-565E-4CC0-BF4C-4C508A7DB46B}"/>
     <hyperlink ref="D49" r:id="rId132" xr:uid="{F21E2C79-F93D-4514-A579-ECA77808FB5C}"/>
+    <hyperlink ref="D68" r:id="rId133" xr:uid="{B6DDFCF8-2D59-4DA8-9C7A-A1B7B7E26168}"/>
+    <hyperlink ref="E68" r:id="rId134" xr:uid="{42C95BBC-98B4-4E80-B097-88E6F392B903}"/>
   </hyperlinks>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6786,16 +6879,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -6807,16 +6900,16 @@
         <v>322</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -6828,16 +6921,16 @@
         <v>148</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6849,16 +6942,16 @@
         <v>139</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -6870,16 +6963,16 @@
         <v>143</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6891,16 +6984,16 @@
         <v>406</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6912,16 +7005,16 @@
         <v>60</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6933,16 +7026,16 @@
         <v>127</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -6954,16 +7047,16 @@
         <v>132</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6975,16 +7068,16 @@
         <v>180</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6996,16 +7089,16 @@
         <v>93</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -7017,16 +7110,16 @@
         <v>100</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -7038,16 +7131,16 @@
         <v>110</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -7059,16 +7152,16 @@
         <v>85</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -7080,16 +7173,16 @@
         <v>417</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -7101,16 +7194,16 @@
         <v>364</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -7122,16 +7215,16 @@
         <v>371</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -7143,16 +7236,16 @@
         <v>153</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -7164,16 +7257,16 @@
         <v>39</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -7185,16 +7278,16 @@
         <v>352</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -7206,16 +7299,16 @@
         <v>60</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -7227,16 +7320,16 @@
         <v>100</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -7248,16 +7341,16 @@
         <v>385</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -7269,16 +7362,16 @@
         <v>148</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -7290,16 +7383,16 @@
         <v>391</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -7311,16 +7404,16 @@
         <v>378</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -7332,16 +7425,16 @@
         <v>396</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -7353,16 +7446,16 @@
         <v>68</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F28" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -7374,16 +7467,16 @@
         <v>401</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -7395,16 +7488,16 @@
         <v>406</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -7416,16 +7509,16 @@
         <v>127</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -7437,16 +7530,16 @@
         <v>364</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -7458,16 +7551,16 @@
         <v>371</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -7479,16 +7572,16 @@
         <v>153</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -7500,16 +7593,16 @@
         <v>39</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -7521,16 +7614,16 @@
         <v>352</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -7542,16 +7635,16 @@
         <v>60</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -7563,16 +7656,16 @@
         <v>100</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -7584,16 +7677,16 @@
         <v>385</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -7605,16 +7698,16 @@
         <v>148</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -7626,16 +7719,16 @@
         <v>391</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -7647,16 +7740,16 @@
         <v>378</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -7668,16 +7761,16 @@
         <v>396</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -7689,16 +7782,16 @@
         <v>68</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -7710,16 +7803,16 @@
         <v>401</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -7731,16 +7824,16 @@
         <v>406</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -7752,16 +7845,16 @@
         <v>127</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -7773,16 +7866,16 @@
         <v>148</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="F48" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -7794,16 +7887,16 @@
         <v>110</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="F49" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -7815,16 +7908,16 @@
         <v>219</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="F50" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -7836,16 +7929,16 @@
         <v>127</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="F51" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -7857,16 +7950,16 @@
         <v>143</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="F52" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -7878,16 +7971,16 @@
         <v>60</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="F53" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -7899,16 +7992,16 @@
         <v>424</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -7920,16 +8013,16 @@
         <v>180</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -7941,16 +8034,16 @@
         <v>265</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -7962,16 +8055,16 @@
         <v>148</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -7983,16 +8076,16 @@
         <v>406</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -8004,16 +8097,16 @@
         <v>127</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F59" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -8025,16 +8118,16 @@
         <v>153</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E60" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F60" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -8046,16 +8139,16 @@
         <v>68</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E61" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F61" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -8067,16 +8160,16 @@
         <v>93</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F62" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -8088,16 +8181,16 @@
         <v>322</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E63" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -8109,16 +8202,16 @@
         <v>371</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E64" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -8130,16 +8223,16 @@
         <v>22</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E65" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -8151,16 +8244,16 @@
         <v>227</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E66" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -8172,16 +8265,16 @@
         <v>396</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E67" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -8193,16 +8286,16 @@
         <v>85</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -8214,16 +8307,16 @@
         <v>378</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E69" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -8235,16 +8328,16 @@
         <v>143</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -8256,16 +8349,16 @@
         <v>75</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -8277,16 +8370,16 @@
         <v>132</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -8298,16 +8391,16 @@
         <v>60</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E73" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -8319,16 +8412,16 @@
         <v>424</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D74" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E74" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F74" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -8340,16 +8433,16 @@
         <v>180</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D75" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E75" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F75" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -8361,16 +8454,16 @@
         <v>265</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D76" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E76" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F76" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -8382,16 +8475,16 @@
         <v>148</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D77" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E77" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F77" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -8403,16 +8496,16 @@
         <v>406</v>
       </c>
       <c r="C78" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D78" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E78" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F78" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -8424,16 +8517,16 @@
         <v>127</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D79" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E79" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F79" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -8445,16 +8538,16 @@
         <v>153</v>
       </c>
       <c r="C80" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D80" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E80" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F80" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -8466,16 +8559,16 @@
         <v>68</v>
       </c>
       <c r="C81" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D81" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E81" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F81" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -8487,16 +8580,16 @@
         <v>93</v>
       </c>
       <c r="C82" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D82" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E82" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F82" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -8508,16 +8601,16 @@
         <v>322</v>
       </c>
       <c r="C83" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D83" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E83" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F83" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -8529,16 +8622,16 @@
         <v>371</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D84" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E84" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F84" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -8550,16 +8643,16 @@
         <v>22</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D85" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E85" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F85" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -8571,16 +8664,16 @@
         <v>227</v>
       </c>
       <c r="C86" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D86" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E86" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F86" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -8592,16 +8685,16 @@
         <v>396</v>
       </c>
       <c r="C87" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D87" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E87" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F87" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -8613,16 +8706,16 @@
         <v>85</v>
       </c>
       <c r="C88" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D88" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E88" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F88" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -8634,16 +8727,16 @@
         <v>378</v>
       </c>
       <c r="C89" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D89" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E89" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F89" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -8655,16 +8748,16 @@
         <v>143</v>
       </c>
       <c r="C90" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D90" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E90" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F90" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -8676,16 +8769,16 @@
         <v>75</v>
       </c>
       <c r="C91" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D91" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E91" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F91" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -8697,16 +8790,16 @@
         <v>132</v>
       </c>
       <c r="C92" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D92" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E92" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F92" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -8718,16 +8811,16 @@
         <v>60</v>
       </c>
       <c r="C93" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D93" s="24" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="E93" s="29" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F93" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="15.75">
@@ -8739,16 +8832,16 @@
         <v>424</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E94" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F94" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="15.75">
@@ -8760,16 +8853,16 @@
         <v>180</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E95" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F95" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="15.75">
@@ -8781,16 +8874,16 @@
         <v>265</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E96" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F96" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="15.75">
@@ -8802,16 +8895,16 @@
         <v>148</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E97" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F97" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="15.75">
@@ -8823,16 +8916,16 @@
         <v>406</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E98" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F98" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="15.75">
@@ -8844,16 +8937,16 @@
         <v>127</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E99" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F99" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="15.75">
@@ -8865,16 +8958,16 @@
         <v>153</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E100" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F100" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="15.75">
@@ -8886,16 +8979,16 @@
         <v>68</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E101" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F101" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="15.75">
@@ -8907,16 +9000,16 @@
         <v>93</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E102" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F102" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="15.75">
@@ -8928,16 +9021,16 @@
         <v>322</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E103" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F103" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="15.75">
@@ -8949,16 +9042,16 @@
         <v>371</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E104" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F104" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="15.75">
@@ -8970,16 +9063,16 @@
         <v>22</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E105" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F105" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="15.75">
@@ -8991,16 +9084,16 @@
         <v>227</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E106" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F106" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="15.75">
@@ -9012,16 +9105,16 @@
         <v>396</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E107" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F107" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="15.75">
@@ -9033,16 +9126,16 @@
         <v>85</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E108" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F108" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="15.75">
@@ -9054,16 +9147,16 @@
         <v>378</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E109" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F109" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="15.75">
@@ -9075,16 +9168,16 @@
         <v>143</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D110" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E110" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F110" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="15.75">
@@ -9096,16 +9189,16 @@
         <v>75</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E111" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F111" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="15.75">
@@ -9117,16 +9210,16 @@
         <v>132</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D112" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E112" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F112" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="15.75">
@@ -9138,16 +9231,16 @@
         <v>60</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="E113" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="F113" s="17" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -9159,16 +9252,16 @@
         <v>410</v>
       </c>
       <c r="C114" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D114" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E114" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F114" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -9180,16 +9273,16 @@
         <v>301</v>
       </c>
       <c r="C115" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D115" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E115" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F115" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -9201,16 +9294,16 @@
         <v>424</v>
       </c>
       <c r="C116" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D116" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E116" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F116" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -9222,16 +9315,16 @@
         <v>431</v>
       </c>
       <c r="C117" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D117" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E117" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F117" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -9243,16 +9336,16 @@
         <v>265</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D118" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E118" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F118" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -9264,16 +9357,16 @@
         <v>203</v>
       </c>
       <c r="C119" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D119" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E119" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F119" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -9285,16 +9378,16 @@
         <v>477</v>
       </c>
       <c r="C120" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D120" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E120" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F120" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -9306,16 +9399,16 @@
         <v>227</v>
       </c>
       <c r="C121" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D121" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E121" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F121" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -9327,16 +9420,16 @@
         <v>406</v>
       </c>
       <c r="C122" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D122" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E122" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F122" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -9348,16 +9441,16 @@
         <v>438</v>
       </c>
       <c r="C123" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D123" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E123" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F123" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -9369,16 +9462,16 @@
         <v>153</v>
       </c>
       <c r="C124" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D124" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E124" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F124" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -9390,16 +9483,16 @@
         <v>444</v>
       </c>
       <c r="C125" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D125" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E125" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F125" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -9411,16 +9504,16 @@
         <v>148</v>
       </c>
       <c r="C126" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D126" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E126" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F126" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -9432,16 +9525,16 @@
         <v>127</v>
       </c>
       <c r="C127" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D127" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E127" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F127" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -9453,16 +9546,16 @@
         <v>451</v>
       </c>
       <c r="C128" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D128" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E128" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F128" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -9474,16 +9567,16 @@
         <v>457</v>
       </c>
       <c r="C129" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D129" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E129" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F129" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -9495,16 +9588,16 @@
         <v>396</v>
       </c>
       <c r="C130" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D130" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E130" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F130" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -9516,16 +9609,16 @@
         <v>465</v>
       </c>
       <c r="C131" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D131" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E131" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F131" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -9537,171 +9630,171 @@
         <v>472</v>
       </c>
       <c r="C132" s="24" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="D132" s="24" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="E132" s="28" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F132" s="27" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="133" spans="1:6">
       <c r="F133" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="F134" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="135" spans="1:6">
       <c r="F135" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="15" customHeight="1">
       <c r="F136" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="15" customHeight="1">
       <c r="F137" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="15" customHeight="1">
       <c r="F138" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="15" customHeight="1">
       <c r="F139" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="140" spans="1:6" ht="15" customHeight="1">
       <c r="F140" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="15" customHeight="1">
       <c r="F141" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="142" spans="1:6" ht="15" customHeight="1">
       <c r="F142" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="15" customHeight="1">
       <c r="F143" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="15" customHeight="1">
       <c r="F144" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="145" spans="6:6" ht="15" customHeight="1">
       <c r="F145" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="146" spans="6:6" ht="15" customHeight="1">
       <c r="F146" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="147" spans="6:6" ht="15" customHeight="1">
       <c r="F147" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="148" spans="6:6" ht="15" customHeight="1">
       <c r="F148" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="149" spans="6:6" ht="15" customHeight="1">
       <c r="F149" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="150" spans="6:6" ht="15" customHeight="1">
       <c r="F150" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="151" spans="6:6" ht="15" customHeight="1">
       <c r="F151" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="152" spans="6:6" ht="15" customHeight="1">
       <c r="F152" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="153" spans="6:6" ht="15" customHeight="1">
       <c r="F153" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="154" spans="6:6" ht="15" customHeight="1">
       <c r="F154" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="155" spans="6:6" ht="15" customHeight="1">
       <c r="F155" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="156" spans="6:6" ht="15" customHeight="1">
       <c r="F156" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="157" spans="6:6" ht="15" customHeight="1">
       <c r="F157" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="158" spans="6:6" ht="15" customHeight="1">
       <c r="F158" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="159" spans="6:6" ht="15" customHeight="1">
       <c r="F159" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="160" spans="6:6" ht="15" customHeight="1">
       <c r="F160" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="161" spans="6:6" ht="15" customHeight="1">
       <c r="F161" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="162" spans="6:6" ht="15" customHeight="1">
       <c r="F162" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="163" spans="6:6" ht="15" customHeight="1">
       <c r="F163" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -9722,20 +9815,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="7855343b-5261-4afc-a17c-d4c130fbaa85" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="7855343b-5261-4afc-a17c-d4c130fbaa85" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9986,11 +10079,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BE4A15A-EC2D-4537-B6DC-2F235DBE6314}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F53F9CFB-0E7D-4BF1-9CBE-0D133C6536E4}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F53F9CFB-0E7D-4BF1-9CBE-0D133C6536E4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BE4A15A-EC2D-4537-B6DC-2F235DBE6314}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>